<commit_message>
Added Tenure without Probation cases
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/Tenure_Leave_Scenarios.xlsx
+++ b/src/main/resources/TestData/Tenure_Leave_Scenarios.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16123" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16206" uniqueCount="366">
   <si>
     <t xml:space="preserve">Test Case</t>
   </si>
@@ -3250,19 +3250,17 @@
   </sheetPr>
   <dimension ref="A1:Z209"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V1" activeCellId="1" sqref="V2:V83 V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.1173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.7857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="102.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19375,21 +19373,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X83"/>
+  <dimension ref="A1:Y83"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V2" activeCellId="0" sqref="V2:V83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="22" min="6" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="14.3112244897959"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19457,12 +19455,15 @@
         <v>20</v>
       </c>
       <c r="V1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -19531,12 +19532,15 @@
         <v>30</v>
       </c>
       <c r="V2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W2" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X2" s="0" t="s">
+      <c r="Y2" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -19605,16 +19609,19 @@
         <v>30</v>
       </c>
       <c r="V3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="X3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X3" s="0" t="s">
+      <c r="Y3" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="102.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="113.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -19679,12 +19686,15 @@
         <v>30</v>
       </c>
       <c r="V4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W4" s="6" t="s">
+      <c r="X4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X4" s="0" t="s">
+      <c r="Y4" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -19753,12 +19763,15 @@
         <v>30</v>
       </c>
       <c r="V5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W5" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W5" s="6" t="s">
+      <c r="X5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X5" s="0" t="s">
+      <c r="Y5" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -19827,12 +19840,15 @@
         <v>30</v>
       </c>
       <c r="V6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W6" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W6" s="6" t="s">
+      <c r="X6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X6" s="0" t="s">
+      <c r="Y6" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -19901,12 +19917,15 @@
         <v>30</v>
       </c>
       <c r="V7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W7" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W7" s="6" t="s">
+      <c r="X7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X7" s="0" t="s">
+      <c r="Y7" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -19975,12 +19994,15 @@
         <v>30</v>
       </c>
       <c r="V8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W8" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W8" s="6" t="s">
+      <c r="X8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X8" s="0" t="s">
+      <c r="Y8" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -20049,16 +20071,19 @@
         <v>27</v>
       </c>
       <c r="V9" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W9" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W9" s="6" t="s">
+      <c r="X9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X9" s="0" t="s">
+      <c r="Y9" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="102.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -20123,12 +20148,15 @@
         <v>30</v>
       </c>
       <c r="V10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W10" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W10" s="6" t="s">
+      <c r="X10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X10" s="0" t="s">
+      <c r="Y10" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -20197,12 +20225,15 @@
         <v>27</v>
       </c>
       <c r="V11" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W11" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W11" s="6" t="s">
+      <c r="X11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X11" s="0" t="s">
+      <c r="Y11" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -20271,12 +20302,15 @@
         <v>30</v>
       </c>
       <c r="V12" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W12" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W12" s="6" t="s">
+      <c r="X12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X12" s="0" t="s">
+      <c r="Y12" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -20345,12 +20379,15 @@
         <v>30</v>
       </c>
       <c r="V13" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W13" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W13" s="6" t="s">
+      <c r="X13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X13" s="0" t="s">
+      <c r="Y13" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -20419,16 +20456,19 @@
         <v>27</v>
       </c>
       <c r="V14" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W14" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W14" s="6" t="s">
+      <c r="X14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X14" s="0" t="s">
+      <c r="Y14" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="136.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="147.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -20493,12 +20533,15 @@
         <v>30</v>
       </c>
       <c r="V15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W15" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W15" s="6" t="s">
+      <c r="X15" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X15" s="0" t="s">
+      <c r="Y15" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -20567,12 +20610,15 @@
         <v>27</v>
       </c>
       <c r="V16" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W16" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W16" s="6" t="s">
+      <c r="X16" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X16" s="0" t="s">
+      <c r="Y16" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -20641,16 +20687,19 @@
         <v>30</v>
       </c>
       <c r="V17" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W17" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W17" s="6" t="s">
+      <c r="X17" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X17" s="0" t="s">
+      <c r="Y17" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="125.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="136.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
@@ -20715,16 +20764,19 @@
         <v>30</v>
       </c>
       <c r="V18" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W18" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W18" s="6" t="s">
+      <c r="X18" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X18" s="0" t="s">
+      <c r="Y18" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="125.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="136.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -20789,16 +20841,19 @@
         <v>27</v>
       </c>
       <c r="V19" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W19" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W19" s="6" t="s">
+      <c r="X19" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X19" s="0" t="s">
+      <c r="Y19" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="125.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="147.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -20863,16 +20918,19 @@
         <v>30</v>
       </c>
       <c r="V20" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W20" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W20" s="6" t="s">
+      <c r="X20" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X20" s="0" t="s">
+      <c r="Y20" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="125.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="136.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -20937,16 +20995,19 @@
         <v>27</v>
       </c>
       <c r="V21" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W21" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W21" s="6" t="s">
+      <c r="X21" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X21" s="0" t="s">
+      <c r="Y21" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="113.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="125.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -21011,12 +21072,15 @@
         <v>30</v>
       </c>
       <c r="V22" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W22" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W22" s="6" t="s">
+      <c r="X22" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X22" s="0" t="s">
+      <c r="Y22" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -21085,12 +21149,15 @@
         <v>30</v>
       </c>
       <c r="V23" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W23" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W23" s="6" t="s">
+      <c r="X23" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X23" s="0" t="s">
+      <c r="Y23" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -21159,16 +21226,19 @@
         <v>27</v>
       </c>
       <c r="V24" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W24" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W24" s="6" t="s">
+      <c r="X24" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X24" s="0" t="s">
+      <c r="Y24" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="125.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="136.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -21233,12 +21303,15 @@
         <v>30</v>
       </c>
       <c r="V25" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W25" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W25" s="6" t="s">
+      <c r="X25" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X25" s="0" t="s">
+      <c r="Y25" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -21307,12 +21380,15 @@
         <v>27</v>
       </c>
       <c r="V26" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W26" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W26" s="6" t="s">
+      <c r="X26" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X26" s="0" t="s">
+      <c r="Y26" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -21381,12 +21457,15 @@
         <v>30</v>
       </c>
       <c r="V27" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W27" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W27" s="6" t="s">
+      <c r="X27" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X27" s="0" t="s">
+      <c r="Y27" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -21455,12 +21534,15 @@
         <v>30</v>
       </c>
       <c r="V28" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W28" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W28" s="6" t="s">
+      <c r="X28" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X28" s="0" t="s">
+      <c r="Y28" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -21529,16 +21611,19 @@
         <v>27</v>
       </c>
       <c r="V29" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W29" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W29" s="6" t="s">
+      <c r="X29" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X29" s="0" t="s">
+      <c r="Y29" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="136.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="147.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -21603,12 +21688,15 @@
         <v>30</v>
       </c>
       <c r="V30" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W30" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W30" s="6" t="s">
+      <c r="X30" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X30" s="0" t="s">
+      <c r="Y30" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -21677,12 +21765,15 @@
         <v>27</v>
       </c>
       <c r="V31" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W31" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W31" s="6" t="s">
+      <c r="X31" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X31" s="0" t="s">
+      <c r="Y31" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -21751,12 +21842,15 @@
         <v>30</v>
       </c>
       <c r="V32" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W32" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W32" s="6" t="s">
+      <c r="X32" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X32" s="0" t="s">
+      <c r="Y32" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -21825,12 +21919,15 @@
         <v>30</v>
       </c>
       <c r="V33" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W33" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W33" s="6" t="s">
+      <c r="X33" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X33" s="0" t="s">
+      <c r="Y33" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -21899,16 +21996,19 @@
         <v>27</v>
       </c>
       <c r="V34" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W34" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W34" s="6" t="s">
+      <c r="X34" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X34" s="0" t="s">
+      <c r="Y34" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="136.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="147.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>25</v>
       </c>
@@ -21973,12 +22073,15 @@
         <v>30</v>
       </c>
       <c r="V35" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W35" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W35" s="6" t="s">
+      <c r="X35" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X35" s="0" t="s">
+      <c r="Y35" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -22047,12 +22150,15 @@
         <v>27</v>
       </c>
       <c r="V36" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W36" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W36" s="6" t="s">
+      <c r="X36" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X36" s="0" t="s">
+      <c r="Y36" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -22121,12 +22227,15 @@
         <v>30</v>
       </c>
       <c r="V37" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W37" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W37" s="6" t="s">
+      <c r="X37" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X37" s="0" t="s">
+      <c r="Y37" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -22195,12 +22304,15 @@
         <v>30</v>
       </c>
       <c r="V38" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W38" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W38" s="6" t="s">
+      <c r="X38" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X38" s="0" t="s">
+      <c r="Y38" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -22269,16 +22381,19 @@
         <v>27</v>
       </c>
       <c r="V39" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W39" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W39" s="6" t="s">
+      <c r="X39" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X39" s="0" t="s">
+      <c r="Y39" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="136.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="147.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>25</v>
       </c>
@@ -22343,12 +22458,15 @@
         <v>30</v>
       </c>
       <c r="V40" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W40" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W40" s="6" t="s">
+      <c r="X40" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X40" s="0" t="s">
+      <c r="Y40" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -22417,12 +22535,15 @@
         <v>27</v>
       </c>
       <c r="V41" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W41" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W41" s="6" t="s">
+      <c r="X41" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X41" s="0" t="s">
+      <c r="Y41" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -22491,12 +22612,15 @@
         <v>30</v>
       </c>
       <c r="V42" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W42" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W42" s="6" t="s">
+      <c r="X42" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X42" s="0" t="s">
+      <c r="Y42" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -22565,12 +22689,15 @@
         <v>30</v>
       </c>
       <c r="V43" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W43" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W43" s="6" t="s">
+      <c r="X43" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X43" s="0" t="s">
+      <c r="Y43" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -22639,16 +22766,19 @@
         <v>30</v>
       </c>
       <c r="V44" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W44" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W44" s="6" t="s">
+      <c r="X44" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X44" s="0" t="s">
+      <c r="Y44" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="102.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="113.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>25</v>
       </c>
@@ -22713,12 +22843,15 @@
         <v>30</v>
       </c>
       <c r="V45" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W45" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W45" s="6" t="s">
+      <c r="X45" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X45" s="0" t="s">
+      <c r="Y45" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -22787,12 +22920,15 @@
         <v>30</v>
       </c>
       <c r="V46" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W46" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W46" s="6" t="s">
+      <c r="X46" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X46" s="0" t="s">
+      <c r="Y46" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -22861,12 +22997,15 @@
         <v>30</v>
       </c>
       <c r="V47" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W47" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W47" s="6" t="s">
+      <c r="X47" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X47" s="0" t="s">
+      <c r="Y47" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -22935,12 +23074,15 @@
         <v>30</v>
       </c>
       <c r="V48" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W48" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W48" s="6" t="s">
+      <c r="X48" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X48" s="0" t="s">
+      <c r="Y48" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -23009,12 +23151,15 @@
         <v>30</v>
       </c>
       <c r="V49" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W49" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W49" s="6" t="s">
+      <c r="X49" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X49" s="0" t="s">
+      <c r="Y49" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -23083,16 +23228,19 @@
         <v>27</v>
       </c>
       <c r="V50" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W50" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W50" s="6" t="s">
+      <c r="X50" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X50" s="0" t="s">
+      <c r="Y50" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="102.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>25</v>
       </c>
@@ -23157,12 +23305,15 @@
         <v>30</v>
       </c>
       <c r="V51" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W51" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W51" s="6" t="s">
+      <c r="X51" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X51" s="0" t="s">
+      <c r="Y51" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -23231,12 +23382,15 @@
         <v>27</v>
       </c>
       <c r="V52" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W52" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W52" s="6" t="s">
+      <c r="X52" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X52" s="0" t="s">
+      <c r="Y52" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -23305,12 +23459,15 @@
         <v>30</v>
       </c>
       <c r="V53" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W53" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W53" s="6" t="s">
+      <c r="X53" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X53" s="0" t="s">
+      <c r="Y53" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -23379,12 +23536,15 @@
         <v>30</v>
       </c>
       <c r="V54" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W54" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W54" s="6" t="s">
+      <c r="X54" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X54" s="0" t="s">
+      <c r="Y54" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -23453,16 +23613,19 @@
         <v>27</v>
       </c>
       <c r="V55" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W55" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W55" s="6" t="s">
+      <c r="X55" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X55" s="0" t="s">
+      <c r="Y55" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="136.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="147.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>25</v>
       </c>
@@ -23527,12 +23690,15 @@
         <v>30</v>
       </c>
       <c r="V56" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W56" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W56" s="6" t="s">
+      <c r="X56" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X56" s="0" t="s">
+      <c r="Y56" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -23601,12 +23767,15 @@
         <v>27</v>
       </c>
       <c r="V57" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W57" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W57" s="6" t="s">
+      <c r="X57" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X57" s="0" t="s">
+      <c r="Y57" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -23675,16 +23844,19 @@
         <v>30</v>
       </c>
       <c r="V58" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W58" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W58" s="6" t="s">
+      <c r="X58" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X58" s="0" t="s">
+      <c r="Y58" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="125.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="136.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>25</v>
       </c>
@@ -23749,16 +23921,19 @@
         <v>30</v>
       </c>
       <c r="V59" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W59" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W59" s="6" t="s">
+      <c r="X59" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X59" s="0" t="s">
+      <c r="Y59" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="125.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="136.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>25</v>
       </c>
@@ -23823,16 +23998,19 @@
         <v>27</v>
       </c>
       <c r="V60" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W60" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W60" s="6" t="s">
+      <c r="X60" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X60" s="0" t="s">
+      <c r="Y60" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="125.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="147.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>25</v>
       </c>
@@ -23897,16 +24075,19 @@
         <v>30</v>
       </c>
       <c r="V61" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W61" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W61" s="6" t="s">
+      <c r="X61" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X61" s="0" t="s">
+      <c r="Y61" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="125.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="136.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>25</v>
       </c>
@@ -23971,16 +24152,19 @@
         <v>27</v>
       </c>
       <c r="V62" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W62" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W62" s="6" t="s">
+      <c r="X62" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X62" s="0" t="s">
+      <c r="Y62" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="113.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="125.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
         <v>25</v>
       </c>
@@ -24045,12 +24229,15 @@
         <v>30</v>
       </c>
       <c r="V63" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W63" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W63" s="6" t="s">
+      <c r="X63" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X63" s="0" t="s">
+      <c r="Y63" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -24119,12 +24306,15 @@
         <v>30</v>
       </c>
       <c r="V64" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W64" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W64" s="6" t="s">
+      <c r="X64" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X64" s="0" t="s">
+      <c r="Y64" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -24193,16 +24383,19 @@
         <v>27</v>
       </c>
       <c r="V65" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W65" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W65" s="6" t="s">
+      <c r="X65" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X65" s="0" t="s">
+      <c r="Y65" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="125.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="136.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
         <v>25</v>
       </c>
@@ -24267,12 +24460,15 @@
         <v>30</v>
       </c>
       <c r="V66" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W66" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W66" s="6" t="s">
+      <c r="X66" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X66" s="0" t="s">
+      <c r="Y66" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -24341,12 +24537,15 @@
         <v>27</v>
       </c>
       <c r="V67" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W67" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W67" s="6" t="s">
+      <c r="X67" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X67" s="0" t="s">
+      <c r="Y67" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -24415,12 +24614,15 @@
         <v>30</v>
       </c>
       <c r="V68" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W68" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W68" s="6" t="s">
+      <c r="X68" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X68" s="0" t="s">
+      <c r="Y68" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -24489,12 +24691,15 @@
         <v>30</v>
       </c>
       <c r="V69" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W69" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W69" s="6" t="s">
+      <c r="X69" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X69" s="0" t="s">
+      <c r="Y69" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -24563,16 +24768,19 @@
         <v>27</v>
       </c>
       <c r="V70" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W70" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W70" s="6" t="s">
+      <c r="X70" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X70" s="0" t="s">
+      <c r="Y70" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="136.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="147.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
         <v>25</v>
       </c>
@@ -24637,12 +24845,15 @@
         <v>30</v>
       </c>
       <c r="V71" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W71" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W71" s="6" t="s">
+      <c r="X71" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X71" s="0" t="s">
+      <c r="Y71" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -24711,12 +24922,15 @@
         <v>27</v>
       </c>
       <c r="V72" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W72" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W72" s="6" t="s">
+      <c r="X72" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X72" s="0" t="s">
+      <c r="Y72" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -24785,12 +24999,15 @@
         <v>30</v>
       </c>
       <c r="V73" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W73" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W73" s="6" t="s">
+      <c r="X73" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X73" s="0" t="s">
+      <c r="Y73" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -24859,12 +25076,15 @@
         <v>30</v>
       </c>
       <c r="V74" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W74" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W74" s="6" t="s">
+      <c r="X74" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X74" s="0" t="s">
+      <c r="Y74" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -24933,16 +25153,19 @@
         <v>27</v>
       </c>
       <c r="V75" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W75" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W75" s="6" t="s">
+      <c r="X75" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X75" s="0" t="s">
+      <c r="Y75" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="136.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="147.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
         <v>25</v>
       </c>
@@ -25007,12 +25230,15 @@
         <v>30</v>
       </c>
       <c r="V76" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W76" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W76" s="6" t="s">
+      <c r="X76" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X76" s="0" t="s">
+      <c r="Y76" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -25081,12 +25307,15 @@
         <v>27</v>
       </c>
       <c r="V77" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W77" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W77" s="6" t="s">
+      <c r="X77" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X77" s="0" t="s">
+      <c r="Y77" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -25155,12 +25384,15 @@
         <v>30</v>
       </c>
       <c r="V78" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W78" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W78" s="6" t="s">
+      <c r="X78" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X78" s="0" t="s">
+      <c r="Y78" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -25229,12 +25461,15 @@
         <v>30</v>
       </c>
       <c r="V79" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W79" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W79" s="6" t="s">
+      <c r="X79" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X79" s="0" t="s">
+      <c r="Y79" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -25303,16 +25538,19 @@
         <v>27</v>
       </c>
       <c r="V80" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W80" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W80" s="6" t="s">
+      <c r="X80" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X80" s="0" t="s">
+      <c r="Y80" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="136.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="147.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
         <v>25</v>
       </c>
@@ -25377,12 +25615,15 @@
         <v>30</v>
       </c>
       <c r="V81" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W81" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W81" s="6" t="s">
+      <c r="X81" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X81" s="0" t="s">
+      <c r="Y81" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -25451,12 +25692,15 @@
         <v>27</v>
       </c>
       <c r="V82" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W82" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W82" s="6" t="s">
+      <c r="X82" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X82" s="0" t="s">
+      <c r="Y82" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -25525,12 +25769,15 @@
         <v>30</v>
       </c>
       <c r="V83" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W83" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="W83" s="6" t="s">
+      <c r="X83" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X83" s="0" t="s">
+      <c r="Y83" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -25553,15 +25800,16 @@
   <dimension ref="A1:U83"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A80" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E85" activeCellId="0" sqref="E85"/>
+      <selection pane="topLeft" activeCell="E85" activeCellId="1" sqref="V2:V83 E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="102.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30978,14 +31226,12 @@
   <dimension ref="A1:U83"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="V2:V83 B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.2857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36402,18 +36648,16 @@
   <dimension ref="A1:Z209"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="V2:V83 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.780612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.4030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52529,13 +52773,10 @@
   <dimension ref="A1:U121"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="V2:V83 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
@@ -60421,12 +60662,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="V2:V83 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Changed scenarios to Run on git
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/Tenure_Leave_Scenarios.xlsx
+++ b/src/main/resources/TestData/Tenure_Leave_Scenarios.xlsx
@@ -17,10 +17,10 @@
     <sheet name="Sheet8" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">All_Without_Probation!$A$1:$Y$83</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">All_Without_Probation!$A$1:$Y$83</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">All_Without_Probation!$A$1:$Y$83</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">All_Without_Probation!$A$1:$Y$83</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">All_Without_Probation!$A$1:$Y$83</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -3249,10 +3249,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -3266,11 +3262,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="102.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19380,24 +19378,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Y83"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="22" min="6" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="6" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="22" min="6" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="6" width="13.0918367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19477,7 +19475,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="68.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -19554,7 +19552,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -19631,7 +19629,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -19708,7 +19706,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -19785,7 +19783,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -19862,7 +19860,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -19947,7 +19945,7 @@
         <v>145</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>241</v>
@@ -20024,7 +20022,7 @@
         <v>146</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>241</v>
@@ -20101,7 +20099,7 @@
         <v>147</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>241</v>
@@ -20170,7 +20168,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -20178,7 +20176,7 @@
         <v>148</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>241</v>
@@ -20255,7 +20253,7 @@
         <v>149</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>241</v>
@@ -20324,7 +20322,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -20401,7 +20399,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -20478,7 +20476,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -20555,7 +20553,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -20632,7 +20630,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -20709,7 +20707,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
@@ -20786,7 +20784,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -20863,7 +20861,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -20940,7 +20938,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -21017,7 +21015,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -21094,7 +21092,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -21171,7 +21169,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -21248,7 +21246,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -21325,7 +21323,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -21402,7 +21400,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -21479,7 +21477,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -21556,7 +21554,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -21633,7 +21631,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -21710,7 +21708,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
@@ -21787,7 +21785,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>25</v>
       </c>
@@ -21864,7 +21862,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>25</v>
       </c>
@@ -21941,7 +21939,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
@@ -22018,7 +22016,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>25</v>
       </c>
@@ -22095,7 +22093,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>25</v>
       </c>
@@ -22172,7 +22170,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>25</v>
       </c>
@@ -22249,7 +22247,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>25</v>
       </c>
@@ -22326,7 +22324,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>25</v>
       </c>
@@ -22403,7 +22401,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>25</v>
       </c>
@@ -22480,7 +22478,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>25</v>
       </c>
@@ -22557,7 +22555,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>25</v>
       </c>
@@ -22634,7 +22632,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="68.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>25</v>
       </c>
@@ -22642,7 +22640,7 @@
         <v>26</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>241</v>
@@ -22711,7 +22709,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>25</v>
       </c>
@@ -22719,7 +22717,7 @@
         <v>34</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>241</v>
@@ -22788,7 +22786,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>25</v>
       </c>
@@ -22796,7 +22794,7 @@
         <v>36</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>241</v>
@@ -22865,7 +22863,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>25</v>
       </c>
@@ -22873,7 +22871,7 @@
         <v>37</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>241</v>
@@ -22942,7 +22940,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>25</v>
       </c>
@@ -22950,7 +22948,7 @@
         <v>38</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>241</v>
@@ -23019,7 +23017,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>25</v>
       </c>
@@ -23027,7 +23025,7 @@
         <v>39</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>241</v>
@@ -23327,7 +23325,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>25</v>
       </c>
@@ -23481,7 +23479,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>25</v>
       </c>
@@ -23489,7 +23487,7 @@
         <v>45</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>241</v>
@@ -23558,7 +23556,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>25</v>
       </c>
@@ -23566,7 +23564,7 @@
         <v>47</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>241</v>
@@ -23635,7 +23633,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>25</v>
       </c>
@@ -23643,7 +23641,7 @@
         <v>49</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>241</v>
@@ -23712,7 +23710,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
         <v>25</v>
       </c>
@@ -23720,7 +23718,7 @@
         <v>51</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>241</v>
@@ -23789,7 +23787,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
         <v>25</v>
       </c>
@@ -23797,7 +23795,7 @@
         <v>53</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>241</v>
@@ -23866,7 +23864,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>25</v>
       </c>
@@ -23874,7 +23872,7 @@
         <v>55</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>241</v>
@@ -23943,7 +23941,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>25</v>
       </c>
@@ -23951,7 +23949,7 @@
         <v>56</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>241</v>
@@ -24020,7 +24018,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>25</v>
       </c>
@@ -24028,7 +24026,7 @@
         <v>57</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>241</v>
@@ -24097,7 +24095,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>25</v>
       </c>
@@ -24105,7 +24103,7 @@
         <v>58</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>241</v>
@@ -24174,7 +24172,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
         <v>25</v>
       </c>
@@ -24182,7 +24180,7 @@
         <v>59</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>241</v>
@@ -24251,7 +24249,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>25</v>
       </c>
@@ -24259,7 +24257,7 @@
         <v>60</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>241</v>
@@ -24328,7 +24326,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
         <v>25</v>
       </c>
@@ -24336,7 +24334,7 @@
         <v>61</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>241</v>
@@ -24405,7 +24403,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
         <v>25</v>
       </c>
@@ -24413,7 +24411,7 @@
         <v>62</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>241</v>
@@ -24482,7 +24480,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
         <v>25</v>
       </c>
@@ -24490,7 +24488,7 @@
         <v>63</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>241</v>
@@ -24559,7 +24557,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
         <v>25</v>
       </c>
@@ -24567,7 +24565,7 @@
         <v>64</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>241</v>
@@ -24636,7 +24634,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
         <v>25</v>
       </c>
@@ -24644,7 +24642,7 @@
         <v>65</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>241</v>
@@ -24713,7 +24711,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
         <v>25</v>
       </c>
@@ -24721,7 +24719,7 @@
         <v>67</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>241</v>
@@ -24790,7 +24788,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
         <v>25</v>
       </c>
@@ -24798,7 +24796,7 @@
         <v>69</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>241</v>
@@ -24867,7 +24865,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
         <v>25</v>
       </c>
@@ -24875,7 +24873,7 @@
         <v>71</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>241</v>
@@ -24944,7 +24942,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
         <v>25</v>
       </c>
@@ -24952,7 +24950,7 @@
         <v>73</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>241</v>
@@ -25021,7 +25019,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
         <v>25</v>
       </c>
@@ -25029,7 +25027,7 @@
         <v>75</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>241</v>
@@ -25098,7 +25096,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
         <v>25</v>
       </c>
@@ -25106,7 +25104,7 @@
         <v>76</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>241</v>
@@ -25175,7 +25173,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
         <v>25</v>
       </c>
@@ -25183,7 +25181,7 @@
         <v>77</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>241</v>
@@ -25252,7 +25250,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
         <v>25</v>
       </c>
@@ -25260,7 +25258,7 @@
         <v>78</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>241</v>
@@ -25329,7 +25327,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
         <v>25</v>
       </c>
@@ -25337,7 +25335,7 @@
         <v>79</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>241</v>
@@ -25406,7 +25404,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
         <v>25</v>
       </c>
@@ -25414,7 +25412,7 @@
         <v>80</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>241</v>
@@ -25483,7 +25481,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
         <v>25</v>
       </c>
@@ -25491,7 +25489,7 @@
         <v>81</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>241</v>
@@ -25560,7 +25558,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
         <v>25</v>
       </c>
@@ -25568,7 +25566,7 @@
         <v>82</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>241</v>
@@ -25637,7 +25635,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
         <v>25</v>
       </c>
@@ -25645,7 +25643,7 @@
         <v>83</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>241</v>
@@ -25714,7 +25712,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
         <v>25</v>
       </c>
@@ -25722,7 +25720,7 @@
         <v>84</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>241</v>
@@ -25792,18 +25790,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Y83">
-    <filterColumn colId="10">
-      <customFilters and="true">
-        <customFilter operator="equal" val="No"/>
-      </customFilters>
-    </filterColumn>
-    <filterColumn colId="15">
-      <customFilters and="true">
-        <customFilter operator="equal" val="Yes"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -25811,7 +25797,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -25828,11 +25813,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="6" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="6" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="102.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31254,7 +31239,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="58.4489795918367"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="57.7755102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36676,11 +36663,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52800,6 +52789,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
@@ -60690,7 +60682,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="6" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="6" width="10.3928571428571"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>